<commit_message>
Updated column headers to csv file, and output to return notes, membership
</commit_message>
<xml_diff>
--- a/Editable Services.xlsx
+++ b/Editable Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BeckettT01\Documents\my_service_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1D08D1C3-1387-4CAF-BD80-1467DB096C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F8EABC-5DD3-48B7-A6BA-D8170891CEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9ACFF3F9-67EC-4D45-B397-9E4537A6CDF5}"/>
   </bookViews>
@@ -22,24 +22,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
-    <t>Membership Cost</t>
-  </si>
-  <si>
     <t>Postcode Areas</t>
   </si>
   <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Phone No.</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -80,6 +71,15 @@
   </si>
   <si>
     <t>https://www.avsed.org.uk/</t>
+  </si>
+  <si>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Membership</t>
   </si>
 </sst>
 </file>
@@ -663,16 +663,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{832F8CDD-6C27-4658-90F9-84F1E6D24E78}" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{832F8CDD-6C27-4658-90F9-84F1E6D24E78}" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:G10" xr:uid="{832F8CDD-6C27-4658-90F9-84F1E6D24E78}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3762080A-CDD8-417A-B3AC-E5E28BF05142}" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{314765AA-CE20-4306-8DAB-FFA40ECECC1E}" name="Categories" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{7B733F30-6123-4127-A710-1749BB2D2071}" name="Membership Cost" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F1C751CB-D32C-48F7-A054-1D094165A970}" name="Postcode Areas" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{3BA0C5A6-7BEF-483E-AE5D-14AD7C78337F}" name="Website" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{D26D7F18-8564-465A-8C7A-4A9783EB3D01}" name="Phone No." dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{4FB6B532-9254-4D81-9C87-AB9BB12E0263}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3762080A-CDD8-417A-B3AC-E5E28BF05142}" name="Service Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{314765AA-CE20-4306-8DAB-FFA40ECECC1E}" name="Categories" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{7B733F30-6123-4127-A710-1749BB2D2071}" name="Membership" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{F1C751CB-D32C-48F7-A054-1D094165A970}" name="Postcode Areas" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{3BA0C5A6-7BEF-483E-AE5D-14AD7C78337F}" name="Website" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D26D7F18-8564-465A-8C7A-4A9783EB3D01}" name="Phone Number" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{4FB6B532-9254-4D81-9C87-AB9BB12E0263}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -998,7 +998,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,62 +1007,62 @@
     <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
     <col min="5" max="5" width="26.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1086,7 +1086,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1098,7 +1098,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>